<commit_message>
Add categories model, controller, tests, and view
</commit_message>
<xml_diff>
--- a/docs/IMS-API.xlsx
+++ b/docs/IMS-API.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15700" yWindow="560" windowWidth="19340" windowHeight="19000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="67">
   <si>
     <t>GET</t>
   </si>
@@ -205,6 +205,21 @@
   </si>
   <si>
     <t>/companies[?search=&lt;name&gt;]</t>
+  </si>
+  <si>
+    <t>CATEGORIES</t>
+  </si>
+  <si>
+    <t>/categories</t>
+  </si>
+  <si>
+    <t>Get complete list of categories</t>
+  </si>
+  <si>
+    <t>/categories/{id}</t>
+  </si>
+  <si>
+    <t>Get information for a specific category</t>
   </si>
 </sst>
 </file>
@@ -384,14 +399,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -411,12 +430,19 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -746,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D40" sqref="A1:D40"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1154,6 +1180,35 @@
         <v>58</v>
       </c>
       <c r="D40" s="18"/>
+    </row>
+    <row r="42" spans="1:4" ht="18">
+      <c r="A42" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D43" s="6"/>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D44" s="21"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>